<commit_message>
Update string-translation Excel files
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
+++ b/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3267C97-02F6-44AB-B527-B79888B4C6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72201444-547A-4FBB-A979-D2D8E9992905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="310">
   <si>
     <t>Key</t>
   </si>
@@ -963,6 +963,15 @@
   </si>
   <si>
     <t>Czech (cs-CZ)</t>
+  </si>
+  <si>
+    <t>strFileHeader29</t>
+  </si>
+  <si>
+    <t>Field description in exported file</t>
+  </si>
+  <si>
+    <t>Differentiation algorithm</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1007,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,8 +1053,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E158" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E158" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E159" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E159" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{15B209E7-880B-40F3-8D04-E1E0C18F3997}" name="Key" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{1492BE55-1C7C-4C02-9979-85AD6633F924}" name="Comment" dataDxfId="2"/>
@@ -1346,7 +1362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99272ECF-2233-463E-857F-E2B1C41A5F55}">
-  <dimension ref="B2:E158"/>
+  <dimension ref="B2:E159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1864,1116 +1880,1128 @@
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1" t="s">
-        <v>100</v>
+      <c r="B50" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>309</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D56" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>163</v>
+        <v>39</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>191</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>191</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>191</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C101" s="1"/>
+        <v>195</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="D101" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>28</v>
+        <v>201</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>211</v>
+        <v>61</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>187</v>
+        <v>220</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C121" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="D121" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C123" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="D123" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1" t="s">
-        <v>102</v>
+        <v>241</v>
       </c>
       <c r="E127" s="1"/>
     </row>
-    <row r="128" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C128" s="1"/>
       <c r="D128" s="1" t="s">
-        <v>244</v>
+        <v>102</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>39</v>
+        <v>252</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>255</v>
+        <v>39</v>
       </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E135" s="1"/>
     </row>
-    <row r="136" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E138" s="1"/>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E138" s="1"/>
-    </row>
-    <row r="139" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B139" s="1" t="s">
+      <c r="E139" s="1"/>
+    </row>
+    <row r="140" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B140" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E139" s="1"/>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="1" t="s">
+      <c r="E140" s="1"/>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="C140" s="1"/>
-      <c r="D140" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E140" s="1"/>
-    </row>
-    <row r="141" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B141" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E141" s="1"/>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C144" s="1"/>
+        <v>273</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="D144" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E147" s="1"/>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>104</v>
+        <v>287</v>
       </c>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
-        <v>290</v>
+        <v>104</v>
       </c>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E158" s="1"/>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E158" s="1"/>
+      <c r="E159" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update integration algorithms strings
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
+++ b/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A3977C-246F-44E0-B02D-387E172C98FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7450F81-1D7E-4F96-8302-0630BF028941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
@@ -1004,9 +1004,6 @@
     <t>strIntegrationAlgorithms</t>
   </si>
   <si>
-    <t>Midpoint rule, Trapezoid rule, Simpson's 1/3 rule</t>
-  </si>
-  <si>
     <t>strFileHeader31</t>
   </si>
   <si>
@@ -1023,6 +1020,9 @@
   </si>
   <si>
     <t>Integration</t>
+  </si>
+  <si>
+    <t>Left-point rule, Mid-point rule, Right-point rule, Trapezoid rule, Simpson's 1/3 rule, Simpson's 3/8 rule, Simpson's composite rule, Romberg's method</t>
   </si>
 </sst>
 </file>
@@ -1975,25 +1975,25 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>97</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>97</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>319</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="E63" s="1"/>
     </row>
@@ -3007,13 +3007,13 @@
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>274</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E153" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update remaining translation files
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
+++ b/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7450F81-1D7E-4F96-8302-0630BF028941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47BA929-970B-4AF0-8149-DC80DC9D9BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="330">
   <si>
     <t>Key</t>
   </si>
@@ -1023,6 +1023,15 @@
   </si>
   <si>
     <t>Left-point rule, Mid-point rule, Right-point rule, Trapezoid rule, Simpson's 1/3 rule, Simpson's 3/8 rule, Simpson's composite rule, Romberg's method</t>
+  </si>
+  <si>
+    <t>strChkAbsoluteIntegral</t>
+  </si>
+  <si>
+    <t>Compute the absolute-value integral?</t>
+  </si>
+  <si>
+    <t>¿Calcular el valor absoluto de la integral?</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1117,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E167" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E167" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E167">
-    <sortCondition ref="B2:B167"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E168" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E168" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E168">
+    <sortCondition ref="B2:B168"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{15B209E7-880B-40F3-8D04-E1E0C18F3997}" name="Key" dataDxfId="3"/>
@@ -1420,7 +1429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99272ECF-2233-463E-857F-E2B1C41A5F55}">
-  <dimension ref="B2:E167"/>
+  <dimension ref="B2:P172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1521,1641 +1530,1661 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>327</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>328</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>318</v>
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>317</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>318</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>316</v>
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>323</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>97</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1" t="s">
-        <v>100</v>
+        <v>320</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>321</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D61" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D64" s="4" t="s">
         <v>326</v>
-      </c>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>314</v>
+        <v>119</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>122</v>
+        <v>312</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>314</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>163</v>
+        <v>39</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>191</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>191</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>191</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C108" s="1"/>
+        <v>195</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="D108" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>28</v>
+        <v>201</v>
       </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>211</v>
+        <v>61</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
-        <v>187</v>
+        <v>220</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C128" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="D128" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="C129" s="1"/>
       <c r="D129" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C130" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="D130" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>102</v>
+        <v>241</v>
       </c>
       <c r="E134" s="1"/>
     </row>
-    <row r="135" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>244</v>
+        <v>102</v>
       </c>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>39</v>
+        <v>252</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>255</v>
+        <v>39</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E143" s="1"/>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E145" s="1"/>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E145" s="1"/>
-    </row>
-    <row r="146" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B146" s="1" t="s">
+      <c r="E146" s="1"/>
+    </row>
+    <row r="147" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D147" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E146" s="1"/>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="1" t="s">
+      <c r="E147" s="1"/>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E147" s="1"/>
-    </row>
-    <row r="148" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B148" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E149" s="1"/>
+    </row>
+    <row r="150" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B150" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C150" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="D150" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="E149" s="1"/>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C152" s="1"/>
+        <v>273</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="D152" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C153" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>325</v>
+        <v>276</v>
+      </c>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C154" s="1"/>
-      <c r="D154" s="1" t="s">
-        <v>279</v>
+        <v>324</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>325</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E158" s="1"/>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>104</v>
+        <v>287</v>
       </c>
       <c r="E159" s="1"/>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>290</v>
+        <v>104</v>
       </c>
       <c r="E160" s="1"/>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E161" s="1"/>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E162" s="1"/>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E163" s="1"/>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E164" s="1"/>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E165" s="1"/>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E166" s="1"/>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E167" s="1"/>
+    </row>
+    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E167" s="1"/>
+      <c r="E168" s="1"/>
+    </row>
+    <row r="172" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N172" t="s">
+        <v>328</v>
+      </c>
+      <c r="P172" t="s">
+        <v>329</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update requested resources files
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
+++ b/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47BA929-970B-4AF0-8149-DC80DC9D9BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BB58C9-A2EF-46F5-9550-066587484D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="332">
   <si>
     <t>Key</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>strChkComputeDerivative</t>
-  </si>
-  <si>
-    <t>In "settings" form</t>
   </si>
   <si>
     <t>Compute numerical differentiation?</t>
@@ -968,9 +965,6 @@
     <t>strFileHeader29</t>
   </si>
   <si>
-    <t>Field description in exported file</t>
-  </si>
-  <si>
     <t>Differentiation algorithm</t>
   </si>
   <si>
@@ -1032,6 +1026,18 @@
   </si>
   <si>
     <t>¿Calcular el valor absoluto de la integral?</t>
+  </si>
+  <si>
+    <t>In "settings" form, tab "Derivative"</t>
+  </si>
+  <si>
+    <t>strFileHeaderColon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: </t>
+  </si>
+  <si>
+    <t>:</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E168" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E168" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E169" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E169" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E168">
     <sortCondition ref="B2:B168"/>
   </sortState>
@@ -1462,10 +1468,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" t="s">
         <v>305</v>
-      </c>
-      <c r="E2" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -1530,13 +1536,13 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1545,1645 +1551,1661 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>99</v>
+        <v>329</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>330</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C62" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="D62" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>326</v>
+        <v>113</v>
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C65" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D65" s="1" t="s">
-        <v>116</v>
+        <v>324</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>313</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>314</v>
+        <v>119</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C69" s="1"/>
+        <v>310</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="D69" s="1" t="s">
-        <v>122</v>
+        <v>312</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>163</v>
+        <v>38</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>98</v>
+        <v>188</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C109" s="1"/>
+        <v>194</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D109" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>204</v>
+        <v>27</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>61</v>
+        <v>207</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>211</v>
+        <v>60</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C126" s="1"/>
       <c r="D126" s="1" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C127" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C129" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="D129" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="C130" s="1"/>
       <c r="D130" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C131" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="D131" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>102</v>
+        <v>240</v>
       </c>
       <c r="E135" s="1"/>
     </row>
-    <row r="136" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>244</v>
+        <v>101</v>
       </c>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E137" s="1"/>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>255</v>
+        <v>38</v>
       </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E143" s="1"/>
     </row>
-    <row r="144" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E144" s="1"/>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E146" s="1"/>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E147" s="1"/>
+    </row>
+    <row r="148" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E146" s="1"/>
-    </row>
-    <row r="147" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B147" s="1" t="s">
+      <c r="C148" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="E148" s="1"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="E147" s="1"/>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E148" s="1"/>
-    </row>
-    <row r="149" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B149" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>265</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="C150" s="4"/>
       <c r="D150" s="4" t="s">
-        <v>311</v>
+        <v>269</v>
       </c>
       <c r="E150" s="1"/>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C151" s="1"/>
+        <v>308</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="D151" s="1" t="s">
-        <v>272</v>
+        <v>309</v>
       </c>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C153" s="1"/>
+        <v>272</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D153" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
-        <v>324</v>
+        <v>275</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>325</v>
+        <v>276</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C155" s="1"/>
+        <v>322</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D155" s="1" t="s">
-        <v>279</v>
+        <v>323</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C156" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D156" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E158" s="1"/>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E159" s="1"/>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>104</v>
+        <v>286</v>
       </c>
       <c r="E160" s="1"/>
     </row>
     <row r="161" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
       <c r="E161" s="1"/>
     </row>
     <row r="162" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E162" s="1"/>
     </row>
     <row r="163" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E163" s="1"/>
     </row>
     <row r="164" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E165" s="1"/>
     </row>
     <row r="166" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E166" s="1"/>
     </row>
     <row r="167" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E167" s="1"/>
     </row>
     <row r="168" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C168" s="1"/>
       <c r="D168" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E168" s="1"/>
+    </row>
+    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E169" s="1"/>
     </row>
     <row r="172" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N172" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P172" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update string-translation Excel books
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
+++ b/SignalAnalysis/localization/Czech (cs-CZ) translation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BB58C9-A2EF-46F5-9550-066587484D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666FBC11-73F2-46C4-937F-615B06D65F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="323">
   <si>
     <t>Key</t>
   </si>
@@ -708,37 +708,10 @@
     <t>strPlotWindowYLabel</t>
   </si>
   <si>
-    <t>strRadBackwardOne</t>
-  </si>
-  <si>
-    <t>In "settings" form, mathematical name</t>
-  </si>
-  <si>
-    <t>Backward one-point difference</t>
-  </si>
-  <si>
-    <t>strRadCentralFive</t>
-  </si>
-  <si>
-    <t>Central five-point difference</t>
-  </si>
-  <si>
-    <t>strRadCentralThree</t>
-  </si>
-  <si>
-    <t>Central three-point difference</t>
-  </si>
-  <si>
     <t>strRadCurrentCulture</t>
   </si>
   <si>
     <t>Current culture formatting</t>
-  </si>
-  <si>
-    <t>strRadForwardOne</t>
-  </si>
-  <si>
-    <t>Forward one-point difference</t>
   </si>
   <si>
     <t>strRadInvariantCulture</t>
@@ -1123,10 +1096,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E169" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E169" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E168">
-    <sortCondition ref="B2:B168"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E165" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E165" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E164">
+    <sortCondition ref="B2:B164"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{15B209E7-880B-40F3-8D04-E1E0C18F3997}" name="Key" dataDxfId="3"/>
@@ -1468,10 +1441,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E2" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -1536,13 +1509,13 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1551,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
@@ -1560,13 +1533,13 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -1615,7 +1588,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>25</v>
@@ -1624,13 +1597,13 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -1990,50 +1963,50 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>96</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -2091,7 +2064,7 @@
         <v>108</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>109</v>
@@ -2120,13 +2093,13 @@
     </row>
     <row r="65" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E65" s="1"/>
     </row>
@@ -2162,13 +2135,13 @@
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E69" s="1"/>
     </row>
@@ -2754,191 +2727,185 @@
       <c r="B127" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="1"/>
+      <c r="D127" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="E132" s="1"/>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E133" s="1"/>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>101</v>
+        <v>240</v>
       </c>
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E137" s="1"/>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="E137" s="1"/>
-    </row>
-    <row r="138" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B138" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>245</v>
+        <v>38</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E140" s="1"/>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>38</v>
+        <v>251</v>
       </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E143" s="1"/>
+    </row>
+    <row r="144" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B144" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E143" s="1"/>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="1" t="s">
+      <c r="C144" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
         <v>256</v>
       </c>
       <c r="E144" s="1"/>
     </row>
-    <row r="145" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
         <v>257</v>
       </c>
@@ -2948,264 +2915,222 @@
       </c>
       <c r="E145" s="1"/>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C146" s="1"/>
-      <c r="D146" s="1" t="s">
+      <c r="C146" s="4"/>
+      <c r="D146" s="4" t="s">
         <v>260</v>
       </c>
       <c r="E146" s="1"/>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E147" s="1"/>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1" t="s">
+      <c r="C148" s="1"/>
+      <c r="D148" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="E147" s="1"/>
-    </row>
-    <row r="148" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B148" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E149" s="1"/>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1" t="s">
+      <c r="C150" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D150" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E149" s="1"/>
-    </row>
-    <row r="150" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B150" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4" t="s">
-        <v>269</v>
-      </c>
       <c r="E150" s="1"/>
     </row>
-    <row r="151" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C152" s="1"/>
+        <v>268</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="D152" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>273</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C154" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>276</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>273</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>280</v>
+        <v>103</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E158" s="1"/>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E159" s="1"/>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E160" s="1"/>
     </row>
     <row r="161" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>103</v>
+        <v>286</v>
       </c>
       <c r="E161" s="1"/>
     </row>
     <row r="162" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E162" s="1"/>
     </row>
     <row r="163" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E163" s="1"/>
     </row>
     <row r="164" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E165" s="1"/>
-    </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B166" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C166" s="1"/>
-      <c r="D166" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E166" s="1"/>
-    </row>
-    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B167" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E167" s="1"/>
-    </row>
-    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B168" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C168" s="1"/>
-      <c r="D168" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E168" s="1"/>
-    </row>
-    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B169" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C169" s="1"/>
-      <c r="D169" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E169" s="1"/>
     </row>
     <row r="172" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N172" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="P172" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>